<commit_message>
Premium User file is added
</commit_message>
<xml_diff>
--- a/target/test-classes/testData/ExcelData.xlsx
+++ b/target/test-classes/testData/ExcelData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE32B032-F4C8-47F8-805C-DAC3B1563825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="9960"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="9" r:id="rId1"/>
+    <sheet name="premiumUser" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="128">
   <si>
     <t>Expected</t>
   </si>
@@ -381,12 +382,30 @@
   </si>
   <si>
     <t>login_28</t>
+  </si>
+  <si>
+    <t>PremiumUser</t>
+  </si>
+  <si>
+    <t>Team01PremiumUser@gmail.com</t>
+  </si>
+  <si>
+    <t>Team01PremiumUser</t>
+  </si>
+  <si>
+    <t>PremiumUserNoData</t>
+  </si>
+  <si>
+    <t>Team01PremiumUserNoData@gmail.com</t>
+  </si>
+  <si>
+    <t>Team01PremiumUserNoData</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,7 +491,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -482,11 +500,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -502,9 +523,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -542,9 +563,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -579,7 +600,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -614,7 +635,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -787,25 +808,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" customWidth="1"/>
+    <col min="3" max="3" width="32.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.53125" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="12" max="12" width="34.109375" customWidth="1"/>
+    <col min="12" max="12" width="34.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -843,7 +864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -854,7 +875,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -868,8 +889,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -879,7 +900,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -893,7 +914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -904,7 +925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -921,7 +942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -941,7 +962,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -961,8 +982,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>72</v>
       </c>
       <c r="G10" t="s">
@@ -981,37 +1002,37 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="8" t="s">
+      <c r="F11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="2"/>
@@ -1028,11 +1049,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="2"/>
@@ -1049,11 +1070,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C14" s="2"/>
@@ -1070,11 +1091,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="2"/>
@@ -1091,11 +1112,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C16" s="2"/>
@@ -1112,11 +1133,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="2"/>
@@ -1133,11 +1154,11 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="2"/>
@@ -1154,11 +1175,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C19" s="2"/>
@@ -1175,11 +1196,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C20" s="2"/>
@@ -1206,11 +1227,11 @@
       </c>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C21" s="2"/>
@@ -1237,21 +1258,21 @@
       </c>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5" t="s">
+      <c r="B22" s="3"/>
+      <c r="C22" s="4" t="s">
         <v>102</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C23" s="2"/>
@@ -1278,11 +1299,11 @@
       </c>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="2"/>
@@ -1309,11 +1330,11 @@
       </c>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C25" s="2"/>
@@ -1340,11 +1361,11 @@
       </c>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C26" s="2"/>
@@ -1371,11 +1392,11 @@
       </c>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C27" s="2"/>
@@ -1402,11 +1423,11 @@
       </c>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C28" s="2"/>
@@ -1435,64 +1456,118 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:12" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>116</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>117</v>
       </c>
       <c r="K29">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>118</v>
       </c>
       <c r="K30" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>121</v>
       </c>
       <c r="K31">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="3"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B5" r:id="rId6"/>
-    <hyperlink ref="B6" r:id="rId7"/>
-    <hyperlink ref="B11" r:id="rId8"/>
-    <hyperlink ref="B12" r:id="rId9"/>
-    <hyperlink ref="B13" r:id="rId10"/>
-    <hyperlink ref="B14" r:id="rId11"/>
-    <hyperlink ref="B15" r:id="rId12"/>
-    <hyperlink ref="B16" r:id="rId13"/>
-    <hyperlink ref="B17" r:id="rId14"/>
-    <hyperlink ref="B18" r:id="rId15"/>
-    <hyperlink ref="B19" r:id="rId16"/>
-    <hyperlink ref="B20" r:id="rId17"/>
-    <hyperlink ref="B21" r:id="rId18"/>
-    <hyperlink ref="B23" r:id="rId19"/>
-    <hyperlink ref="B24" r:id="rId20"/>
-    <hyperlink ref="B25" r:id="rId21"/>
-    <hyperlink ref="B26" r:id="rId22"/>
-    <hyperlink ref="B27" r:id="rId23"/>
-    <hyperlink ref="B28" r:id="rId24"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId25"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{158EE381-6834-486C-9C8E-C5475F45FEA8}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="19.73046875" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="33.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="mailto:Team01PremiumUser@gmail.com" xr:uid="{9DFBBAEB-79A5-4E03-A83C-FF2A20B6A131}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{2CCF3092-F31E-4907-8A55-9F84ECE10DD5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>